<commit_message>
Ajuste if 2-desbloquearPosicoes.cy.js  e 2A-bloquearPosicoes.cy.js
</commit_message>
<xml_diff>
--- a/cypress/fixtures/auto.xlsx
+++ b/cypress/fixtures/auto.xlsx
@@ -8,31 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\MPCE_Atomações_Cypress\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6B71E8-12B8-448A-9E99-031CEE1BC05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BB5368-05B0-4D69-8378-56B198F25273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2-desbloquearposicoes" sheetId="2" r:id="rId1"/>
-    <sheet name="2A-bloquearposicoes" sheetId="3" r:id="rId2"/>
-    <sheet name="3-encerrarNomeacao" sheetId="4" r:id="rId3"/>
-    <sheet name="4-publicVagaEstagio" sheetId="5" r:id="rId4"/>
+    <sheet name="2-desbloquearposicoes" sheetId="1" r:id="rId1"/>
+    <sheet name="2A-bloquearposicoes" sheetId="2" r:id="rId2"/>
+    <sheet name="3-encerrarNomeacao" sheetId="3" r:id="rId3"/>
+    <sheet name="4-publicVagaEstagio" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
-  <si>
-    <t>Estagiário (ID-7)</t>
-  </si>
-  <si>
-    <t>Estagiário (ID-6)</t>
-  </si>
-  <si>
-    <t/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Icaro Santiago</t>
   </si>
@@ -41,6 +32,12 @@
   </si>
   <si>
     <t>Jonatas Gomes</t>
+  </si>
+  <si>
+    <t>Estagiário (ID-7)</t>
+  </si>
+  <si>
+    <t>Estagiário (ID-6)</t>
   </si>
 </sst>
 </file>
@@ -76,9 +73,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,14 +376,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -397,48 +393,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -446,14 +426,14 @@
     <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -462,7 +442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -477,38 +457,35 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inclusao de teste portal 5-demInteresseVagaPortal.cy.js
</commit_message>
<xml_diff>
--- a/cypress/fixtures/auto.xlsx
+++ b/cypress/fixtures/auto.xlsx
@@ -8,29 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\MPCE_Atomações_Cypress\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BB5368-05B0-4D69-8378-56B198F25273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F635EC23-E9BD-4FE1-8CC6-B7929D3A9F53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="3600" windowWidth="20640" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2-desbloquearposicoes" sheetId="1" r:id="rId1"/>
     <sheet name="2A-bloquearposicoes" sheetId="2" r:id="rId2"/>
     <sheet name="3-encerrarNomeacao" sheetId="3" r:id="rId3"/>
     <sheet name="4-publicVagaEstagio" sheetId="4" r:id="rId4"/>
+    <sheet name="5-demonstrInteressVaga" sheetId="5" r:id="rId5"/>
+    <sheet name="5-demInteresseVagaPortal" sheetId="6" r:id="rId6"/>
+    <sheet name="Planilha1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+  <si>
+    <t>Reinaldo Santos</t>
+  </si>
   <si>
     <t>Icaro Santiago</t>
   </si>
   <si>
-    <t>Reinaldo Santos</t>
-  </si>
-  <si>
     <t>Jonatas Gomes</t>
   </si>
   <si>
@@ -38,16 +41,42 @@
   </si>
   <si>
     <t>Estagiário (ID-6)</t>
+  </si>
+  <si>
+    <t>icaro@veloxmail.com.br</t>
+  </si>
+  <si>
+    <t>hfxqt3jg</t>
+  </si>
+  <si>
+    <t>reinaldo@transmazza.com.br</t>
+  </si>
+  <si>
+    <t>flmehms7</t>
+  </si>
+  <si>
+    <t>jonatasteste@teste.com.br</t>
+  </si>
+  <si>
+    <t>yuqzvejf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -70,13 +99,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -382,9 +414,7 @@
   </sheetPr>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -417,9 +447,7 @@
   </sheetPr>
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -463,7 +491,9 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -472,12 +502,12 @@
   <sheetData>
     <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -488,4 +518,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{9681D32A-7741-4FE5-B50C-E5E3B807ACB0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{948CBE9C-E669-4AE4-8BE7-C089E30ABFC6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{74D50072-4DB1-4E4C-B1E6-1A38B7C8D60E}"/>
+    <hyperlink ref="A1" r:id="rId2" xr:uid="{FAD985CC-07F4-4070-B002-DA215140B1EF}"/>
+  </hyperlinks>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>